<commit_message>
added Dashboard first Page of predictive analysis
</commit_message>
<xml_diff>
--- a/Predictive Analysis Dashboard/Customer_Master_Data.xlsx
+++ b/Predictive Analysis Dashboard/Customer_Master_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RUPASREE\Desktop\PREDICTIVE ANALYTICS ON HEALTHCARE\DATASET_OCT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Neha\kaggle Projects\Git hub\PowerBI_Dashboard\Predictive Analysis Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05F671F7-A383-4856-9B5F-A0AAEADAE4DF}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11496A5B-51F9-42FA-8B32-D6FB69BD4799}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0AFCB63E-E906-4689-9A08-EA6AA116A312}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{0AFCB63E-E906-4689-9A08-EA6AA116A312}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer" sheetId="3" r:id="rId1"/>
@@ -22,11 +22,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -128,7 +123,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,12 +133,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -170,10 +159,7 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -564,19 +550,19 @@
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="F5" sqref="F5"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.6640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.08984375" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.6328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -593,8 +579,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -610,8 +596,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -627,8 +613,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" s="6" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="5" t="s">
         <v>15</v>
       </c>
       <c r="B4" s="3" t="s">
@@ -644,8 +630,8 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="6" t="s">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="5" t="s">
         <v>19</v>
       </c>
       <c r="B5" s="3" t="s">

</xml_diff>